<commit_message>
Makefile: correct classpath for JOPtimizer (BCEL 5.2 class loading bug)
</commit_message>
<xml_diff>
--- a/doc/perf.xlsx
+++ b/doc/perf.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="108" windowWidth="15120" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="compare" sheetId="1" r:id="rId1"/>
@@ -167,28 +167,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.16425914295376587</c:v>
+                  <c:v>0.14132513093357718</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.47794579448282526</c:v>
+                  <c:v>0.41121456480172913</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.55896420116913859</c:v>
+                  <c:v>0.48092110732396709</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.68351128073819989</c:v>
+                  <c:v>0.58807880954360292</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1504420503405961</c:v>
+                  <c:v>0.98981627732978639</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9199961350789894</c:v>
+                  <c:v>1.6519245157535956</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.0884583796318661</c:v>
+                  <c:v>1.7968659073904729</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -247,28 +247,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.16205704407951599</c:v>
+                  <c:v>0.14787066246056782</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.31136560069144337</c:v>
+                  <c:v>0.28410883280757099</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.62273120138288673</c:v>
+                  <c:v>0.56821766561514198</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.69306395851339675</c:v>
+                  <c:v>0.63239353312302837</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2910544511668107</c:v>
+                  <c:v>1.1780362776025237</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9124891961970614</c:v>
+                  <c:v>1.7450709779179812</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.2527009507346587</c:v>
+                  <c:v>1.1430402208201893</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -333,7 +333,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.58205189240656985</c:v>
+                  <c:v>0.50296198782293899</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -342,10 +342,10 @@
                   <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2113306355629612</c:v>
+                  <c:v>1.0467335856508146</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.8298976434182337</c:v>
+                  <c:v>1.5812489715320059</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -354,24 +354,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="64334080"/>
-        <c:axId val="64352256"/>
+        <c:axId val="63875328"/>
+        <c:axId val="63889408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="64334080"/>
+        <c:axId val="63875328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64352256"/>
+        <c:crossAx val="63889408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64352256"/>
+        <c:axId val="63889408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -397,7 +397,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64334080"/>
+        <c:crossAx val="63875328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -415,7 +415,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup paperSize="9" orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
@@ -495,7 +495,7 @@
                   <c:v>14148</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>20699</c:v>
+                  <c:v>24058</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>23813</c:v>
@@ -575,7 +575,7 @@
                   <c:v>6415</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9256</c:v>
+                  <c:v>10144</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>11950</c:v>
@@ -646,7 +646,7 @@
                   <c:v>12226</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21005</c:v>
+                  <c:v>24308</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>25444</c:v>
@@ -658,24 +658,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="64587264"/>
-        <c:axId val="64588800"/>
+        <c:axId val="64448000"/>
+        <c:axId val="64449536"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="64587264"/>
+        <c:axId val="64448000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64588800"/>
+        <c:crossAx val="64449536"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="64588800"/>
+        <c:axId val="64449536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -706,7 +706,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="64587264"/>
+        <c:crossAx val="64448000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -719,7 +719,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
     <c:pageSetup orientation="portrait"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1421,11 +1421,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="65409024"/>
-        <c:axId val="67422080"/>
+        <c:axId val="64537344"/>
+        <c:axId val="64538880"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="65409024"/>
+        <c:axId val="64537344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="38353"/>
@@ -1434,7 +1434,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="yyyy" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="67422080"/>
+        <c:crossAx val="64538880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1444,7 +1444,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="67422080"/>
+        <c:axId val="64538880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1475,7 +1475,7 @@
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="65409024"/>
+        <c:crossAx val="64537344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1488,7 +1488,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>
   </c:printSettings>
 </c:chartSpace>
@@ -1739,13 +1739,12 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:dLbls/>
         <c:marker val="1"/>
-        <c:axId val="104635008"/>
-        <c:axId val="104651776"/>
+        <c:axId val="64583936"/>
+        <c:axId val="64589824"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="104635008"/>
+        <c:axId val="64583936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="38353"/>
@@ -1754,7 +1753,7 @@
         <c:minorGridlines/>
         <c:numFmt formatCode="yyyy" sourceLinked="0"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104651776"/>
+        <c:crossAx val="64589824"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
@@ -1764,7 +1763,7 @@
         <c:minorTimeUnit val="months"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="104651776"/>
+        <c:axId val="64589824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1772,7 +1771,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104635008"/>
+        <c:crossAx val="64583936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1781,7 +1780,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup orientation="landscape" horizontalDpi="1200" verticalDpi="1200"/>
   </c:printSettings>
 </c:chartSpace>
@@ -2204,8 +2203,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
@@ -2253,7 +2252,7 @@
         <v>14148</v>
       </c>
       <c r="F2">
-        <v>20699</v>
+        <v>24058</v>
       </c>
       <c r="G2">
         <v>23813</v>
@@ -2282,7 +2281,7 @@
         <v>6415</v>
       </c>
       <c r="F3">
-        <v>9256</v>
+        <v>10144</v>
       </c>
       <c r="G3">
         <v>11950</v>
@@ -2302,7 +2301,7 @@
         <v>12226</v>
       </c>
       <c r="F4">
-        <v>21005</v>
+        <v>24308</v>
       </c>
       <c r="G4">
         <v>25444</v>
@@ -2343,19 +2342,19 @@
       </c>
       <c r="B7">
         <f t="shared" ref="B7:H9" si="0">B2/$F2</f>
-        <v>0.16425914295376587</v>
+        <v>0.14132513093357718</v>
       </c>
       <c r="C7">
         <f t="shared" si="0"/>
-        <v>0.47794579448282526</v>
+        <v>0.41121456480172913</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0.55896420116913859</v>
+        <v>0.48092110732396709</v>
       </c>
       <c r="E7">
         <f t="shared" si="0"/>
-        <v>0.68351128073819989</v>
+        <v>0.58807880954360292</v>
       </c>
       <c r="F7">
         <f t="shared" si="0"/>
@@ -2363,15 +2362,15 @@
       </c>
       <c r="G7">
         <f t="shared" si="0"/>
-        <v>1.1504420503405961</v>
+        <v>0.98981627732978639</v>
       </c>
       <c r="H7">
         <f t="shared" si="0"/>
-        <v>1.9199961350789894</v>
+        <v>1.6519245157535956</v>
       </c>
       <c r="I7">
         <f t="shared" ref="I7" si="1">I2/$F2</f>
-        <v>2.0884583796318661</v>
+        <v>1.7968659073904729</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -2380,19 +2379,19 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>0.16205704407951599</v>
+        <v>0.14787066246056782</v>
       </c>
       <c r="C8">
         <f t="shared" si="0"/>
-        <v>0.31136560069144337</v>
+        <v>0.28410883280757099</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0.62273120138288673</v>
+        <v>0.56821766561514198</v>
       </c>
       <c r="E8">
         <f t="shared" si="0"/>
-        <v>0.69306395851339675</v>
+        <v>0.63239353312302837</v>
       </c>
       <c r="F8">
         <f t="shared" si="0"/>
@@ -2400,15 +2399,15 @@
       </c>
       <c r="G8">
         <f t="shared" si="0"/>
-        <v>1.2910544511668107</v>
+        <v>1.1780362776025237</v>
       </c>
       <c r="H8">
         <f t="shared" si="0"/>
-        <v>1.9124891961970614</v>
+        <v>1.7450709779179812</v>
       </c>
       <c r="I8">
         <f t="shared" ref="I8" si="2">I3/$F3</f>
-        <v>1.2527009507346587</v>
+        <v>1.1430402208201893</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -2425,7 +2424,7 @@
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.58205189240656985</v>
+        <v>0.50296198782293899</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
@@ -2437,11 +2436,11 @@
       </c>
       <c r="G9">
         <f t="shared" si="0"/>
-        <v>1.2113306355629612</v>
+        <v>1.0467335856508146</v>
       </c>
       <c r="H9">
         <f t="shared" si="0"/>
-        <v>1.8298976434182337</v>
+        <v>1.5812489715320059</v>
       </c>
       <c r="I9">
         <f t="shared" ref="I9" si="3">I4/$F4</f>
@@ -2459,7 +2458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N19" sqref="N19"/>
     </sheetView>
   </sheetViews>

</xml_diff>